<commit_message>
buang index aspek betulin db conection di aspek
</commit_message>
<xml_diff>
--- a/Data CSV/group_instansi.xlsx
+++ b/Data CSV/group_instansi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELAINE\ta_elaine\Data CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python_app\ta_elaine\Data CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF04C0CE-0AE0-4AA6-8149-65187E752667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509D198F-804A-4F43-AFEE-0916F97B4F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="345" windowWidth="20310" windowHeight="14205" activeTab="2" xr2:uid="{9603F020-9C66-4CC6-880B-AADE8A662A72}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9603F020-9C66-4CC6-880B-AADE8A662A72}"/>
   </bookViews>
   <sheets>
     <sheet name="grup_instansi" sheetId="1" r:id="rId1"/>
@@ -25,23 +25,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="234">
   <si>
     <t>id</t>
   </si>
@@ -539,13 +528,217 @@
   </si>
   <si>
     <t>INSERT INTO `isi`(`instansi`, `indikator`, `value`, `year`) VALUES</t>
+  </si>
+  <si>
+    <t>gurp</t>
+  </si>
+  <si>
+    <t>Kementerian Koordinator Bidang Pembangunan Manusia dan Kebudayaan</t>
+  </si>
+  <si>
+    <t>Kementerian Koperasi dan Usaha Kecil dan Menengah</t>
+  </si>
+  <si>
+    <t>Kementerian Pemberdayaan Perempuan dan Perlindungan Anak</t>
+  </si>
+  <si>
+    <t>Kementerian Dalam Negeri</t>
+  </si>
+  <si>
+    <t>Kementerian Luar Negeri</t>
+  </si>
+  <si>
+    <t>Kementerian Hukum dan Hak Asasi Manusia</t>
+  </si>
+  <si>
+    <t>Kementerian Pertanian</t>
+  </si>
+  <si>
+    <t>Kementerian Energi dan Sumber Daya Mineral</t>
+  </si>
+  <si>
+    <t>Kementerian Perhubungan</t>
+  </si>
+  <si>
+    <t>Kementerian Ketenagakerjaan</t>
+  </si>
+  <si>
+    <t>Kementerian Perdagangan</t>
+  </si>
+  <si>
+    <t>Kementerian Agraria dan Tata Ruang/Badan Pertanahan Nasional</t>
+  </si>
+  <si>
+    <t>Kementerian Koordinator Bidang Perekonomian</t>
+  </si>
+  <si>
+    <t>Kementerian Koordinator Bidang Kemaritiman</t>
+  </si>
+  <si>
+    <t>Kementerian Badan Usaha Milik Negara</t>
+  </si>
+  <si>
+    <t>Kementerian Pendayagunaan Aparatur Negara dan Reformasi Birokrasi</t>
+  </si>
+  <si>
+    <t>Kementerian Desa, Pembangunan Daerah Tertinggal dan Transmigrasi</t>
+  </si>
+  <si>
+    <t>Kementerian Keuangan</t>
+  </si>
+  <si>
+    <t>Kementerian Pendidikan dan Kebudayaan</t>
+  </si>
+  <si>
+    <t>Kementerian Kesehatan</t>
+  </si>
+  <si>
+    <t>Kementerian Agama</t>
+  </si>
+  <si>
+    <t>Kementerian Sosial</t>
+  </si>
+  <si>
+    <t>Kementerian Lingkungan Hidup dan Kehutanan</t>
+  </si>
+  <si>
+    <t>Kementerian Kelautan dan Perikanan</t>
+  </si>
+  <si>
+    <t>Kementerian Komunikasi dan Informatika</t>
+  </si>
+  <si>
+    <t>Kementerian Pekerjaan Umum &amp; Perumahan Rakyat</t>
+  </si>
+  <si>
+    <t>Kementerian Pariwisata dan Ekonomi Kreatif/Badan Pariwisata dan Ekonomi Kreatif</t>
+  </si>
+  <si>
+    <t>Kementerian Sekretariat Negara</t>
+  </si>
+  <si>
+    <t>Kementerian Perencanaan Pembangunan Nasional/Badan Perencanaan Pembangunan Nasional</t>
+  </si>
+  <si>
+    <t>Kementerian Investasi/Badan Koordinasi Penanaman Modal</t>
+  </si>
+  <si>
+    <t>Kementerian Koordinator Bidang Politik, Hukum dan Keamanan</t>
+  </si>
+  <si>
+    <t>Kementerian Pemuda dan Olahraga</t>
+  </si>
+  <si>
+    <t>Kementerian Pertahanan</t>
+  </si>
+  <si>
+    <t>Kementerian Perindustrian</t>
+  </si>
+  <si>
+    <t>Badan Pembinaan Ideologi Pancasila</t>
+  </si>
+  <si>
+    <t>Badan Intelijen Negara</t>
+  </si>
+  <si>
+    <t>Majelis Permusyawaratan Rakyat</t>
+  </si>
+  <si>
+    <t>Dewan Perwakilan Rakyat</t>
+  </si>
+  <si>
+    <t>Komisi Yudisial</t>
+  </si>
+  <si>
+    <t>Dewan Perwakilan Daerah</t>
+  </si>
+  <si>
+    <t>Radio Republik Indonesia</t>
+  </si>
+  <si>
+    <t>Markas Besar Kepolisian Republik Indonesia</t>
+  </si>
+  <si>
+    <t>Kejaksaan Agung</t>
+  </si>
+  <si>
+    <t>Mahkamah Agung RI</t>
+  </si>
+  <si>
+    <t>Badan Pemeriksa Keuangan</t>
+  </si>
+  <si>
+    <t>Sekretariat Kabinet</t>
+  </si>
+  <si>
+    <t>Mahkamah Konstitusi</t>
+  </si>
+  <si>
+    <t>Televisi Republik Indonesia</t>
+  </si>
+  <si>
+    <t>Dewan Ketahanan Nasional</t>
+  </si>
+  <si>
+    <t>Komisi Pemilihan Umum</t>
+  </si>
+  <si>
+    <t>Komisi Pemberantasan Korupsi</t>
+  </si>
+  <si>
+    <t>Pusat Pelaporan dan Analisis Transaksi Keuangan</t>
+  </si>
+  <si>
+    <t>Ombudsman Republik Indonesia</t>
+  </si>
+  <si>
+    <t>Badan Nasional Pengelola Perbatasan</t>
+  </si>
+  <si>
+    <t>Komisi Aparatur Sipil Negara</t>
+  </si>
+  <si>
+    <t>Badan Amil Zakat Nasional</t>
+  </si>
+  <si>
+    <t>Komisi Pengawas Persaingan Usaha</t>
+  </si>
+  <si>
+    <t>Badan Pengawas Pemilihan Umum</t>
+  </si>
+  <si>
+    <t>Komisi Penyiaran Indonesia</t>
+  </si>
+  <si>
+    <t>Komisi Informasi Pusat</t>
+  </si>
+  <si>
+    <t>Komisi Kejaksaan</t>
+  </si>
+  <si>
+    <t>Dewan Pers</t>
+  </si>
+  <si>
+    <t>Dewan Jaminan Sosial Nasional</t>
+  </si>
+  <si>
+    <t>Lembaga Perlindungan Saksi Dan Korban</t>
+  </si>
+  <si>
+    <t>Lembaga Sensor Film</t>
+  </si>
+  <si>
+    <t>Konsil Kedokteran Indonesia</t>
+  </si>
+  <si>
+    <t>Kantor Staf Presiden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,6 +762,16 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -587,17 +790,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{FF8D6C84-28C9-43B5-857A-6BC49C5FD888}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -912,7 +1118,7 @@
   <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,12 +2315,902 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06365F83-EE82-4A4F-85D6-D04380E57CAA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>"i20231106"&amp;RIGHT(TEXT("G00000"&amp;(ROW(A2)-ROW($A$1)),"0"),5)</f>
+        <v>i2023110600001</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A66" si="0">"i20231106"&amp;RIGHT(TEXT("G00000"&amp;(ROW(A3)-ROW($A$1)),"0"),5)</f>
+        <v>i2023110600002</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600003</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600004</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600005</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600006</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600007</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600008</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600009</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600010</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600011</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600012</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600013</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600014</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600015</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600016</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600017</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600018</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600019</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600020</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C21" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600021</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600022</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600023</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600024</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600025</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600026</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C27" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600027</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600028</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600029</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600030</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C31" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600031</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C32" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600032</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C33" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600033</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C34" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600034</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C35" t="str">
+        <f>grup_instansi!$A$2</f>
+        <v>gi2023110400001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600035</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C36" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600036</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600037</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C38" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600038</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C39" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600039</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C40" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600040</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C41" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600041</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C42" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600042</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C43" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600043</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C44" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600044</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C45" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600045</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C46" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600046</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600047</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600048</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C49" t="str">
+        <f>grup_instansi!$A$3</f>
+        <v>gi2023110400002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600049</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C50" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600050</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C51" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600051</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C52" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600052</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C53" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600053</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C54" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600054</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C55" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600055</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C56" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600056</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C57" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600057</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C58" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600058</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C59" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600059</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C60" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600060</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C61" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600061</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C62" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600062</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C63" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600063</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C64" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600064</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C65" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="str">
+        <f t="shared" si="0"/>
+        <v>i2023110600065</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C66" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f t="shared" ref="A67:A68" si="1">"i20231106"&amp;RIGHT(TEXT("G00000"&amp;(ROW(A67)-ROW($A$1)),"0"),5)</f>
+        <v>i2023110600066</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C67" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="str">
+        <f t="shared" si="1"/>
+        <v>i2023110600067</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C68" t="str">
+        <f>grup_instansi!$A$4</f>
+        <v>gi2023110400003</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2123,7 +3219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E260E74E-0EDD-48AC-B8A8-DF71CA27A0DF}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>